<commit_message>
Finished MCP graphics. Needed to move around various gauges/switches inside MCP. Updated schedule.
</commit_message>
<xml_diff>
--- a/GUIs/todo.xlsx
+++ b/GUIs/todo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saad/Desktop/nasaDataViz/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saad/Desktop/nasaDataViz/NASA/GUIs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCBB8440-FD27-CD46-A50D-B4F96B5C9300}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C56D9F8-73D5-044B-96AE-5B5E7F33720F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18800" yWindow="460" windowWidth="10000" windowHeight="16240" xr2:uid="{18DB9649-71BC-4344-B476-FE1CADB6EB15}"/>
+    <workbookView xWindow="8240" yWindow="460" windowWidth="20560" windowHeight="16240" xr2:uid="{18DB9649-71BC-4344-B476-FE1CADB6EB15}"/>
   </bookViews>
   <sheets>
     <sheet name="MCP" sheetId="1" r:id="rId1"/>
@@ -781,7 +781,7 @@
   <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Finished MCP front-end, able to change memory values in MCP_Sim object and re-render the panel to update values.
</commit_message>
<xml_diff>
--- a/GUIs/todo.xlsx
+++ b/GUIs/todo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saad/Desktop/nasaDataViz/NASA/GUIs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C56D9F8-73D5-044B-96AE-5B5E7F33720F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7695B8D7-2952-2F4F-B853-37C8EF743FC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8240" yWindow="460" windowWidth="20560" windowHeight="16240" xr2:uid="{18DB9649-71BC-4344-B476-FE1CADB6EB15}"/>
+    <workbookView xWindow="17060" yWindow="460" windowWidth="11740" windowHeight="16220" xr2:uid="{18DB9649-71BC-4344-B476-FE1CADB6EB15}"/>
   </bookViews>
   <sheets>
     <sheet name="MCP" sheetId="1" r:id="rId1"/>
@@ -359,7 +359,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -388,14 +388,8 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -418,12 +412,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -454,7 +442,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -463,7 +451,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -781,7 +768,7 @@
   <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -828,7 +815,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="7"/>
+      <c r="A4" s="5"/>
       <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
@@ -850,7 +837,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="8"/>
+      <c r="A5" s="5"/>
       <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
@@ -872,7 +859,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="8"/>
+      <c r="A6" s="5"/>
       <c r="B6" s="4" t="s">
         <v>1</v>
       </c>
@@ -890,7 +877,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="8"/>
+      <c r="A7" s="5"/>
       <c r="B7" s="4" t="s">
         <v>2</v>
       </c>
@@ -908,7 +895,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="8"/>
+      <c r="A8" s="5"/>
       <c r="B8" s="4" t="s">
         <v>20</v>
       </c>
@@ -926,7 +913,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="8"/>
+      <c r="A9" s="5"/>
       <c r="B9" s="4" t="s">
         <v>21</v>
       </c>
@@ -944,7 +931,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="8"/>
+      <c r="A10" s="5"/>
       <c r="B10" s="4" t="s">
         <v>22</v>
       </c>
@@ -962,7 +949,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="7"/>
+      <c r="A11" s="5"/>
       <c r="B11" s="4" t="s">
         <v>23</v>
       </c>
@@ -980,7 +967,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="8"/>
+      <c r="A12" s="5"/>
       <c r="B12" s="4" t="s">
         <v>24</v>
       </c>
@@ -998,7 +985,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="8"/>
+      <c r="A13" s="5"/>
       <c r="B13" s="4" t="s">
         <v>25</v>
       </c>
@@ -1016,7 +1003,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="8"/>
+      <c r="A14" s="5"/>
       <c r="B14" s="4" t="s">
         <v>26</v>
       </c>
@@ -1034,7 +1021,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="8"/>
+      <c r="A15" s="5"/>
       <c r="B15" s="4" t="s">
         <v>27</v>
       </c>
@@ -1052,7 +1039,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="8"/>
+      <c r="A16" s="5"/>
       <c r="B16" s="4" t="s">
         <v>28</v>
       </c>
@@ -1070,7 +1057,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="8"/>
+      <c r="A17" s="5"/>
       <c r="B17" s="4" t="s">
         <v>29</v>
       </c>
@@ -1088,7 +1075,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="8"/>
+      <c r="A18" s="5"/>
       <c r="B18" s="4" t="s">
         <v>30</v>
       </c>
@@ -1106,7 +1093,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="8"/>
+      <c r="A19" s="5"/>
       <c r="B19" s="4" t="s">
         <v>31</v>
       </c>
@@ -1124,7 +1111,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="8"/>
+      <c r="A20" s="5"/>
       <c r="B20" s="4" t="s">
         <v>32</v>
       </c>
@@ -1142,7 +1129,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="8"/>
+      <c r="A21" s="5"/>
       <c r="B21" s="4" t="s">
         <v>33</v>
       </c>
@@ -1160,7 +1147,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="8"/>
+      <c r="A22" s="5"/>
       <c r="B22" s="4" t="s">
         <v>51</v>
       </c>
@@ -1178,7 +1165,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="8"/>
+      <c r="A23" s="5"/>
       <c r="B23" s="4" t="s">
         <v>52</v>
       </c>
@@ -1196,7 +1183,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="7"/>
+      <c r="A24" s="5"/>
       <c r="B24" s="4" t="s">
         <v>53</v>
       </c>
@@ -1214,7 +1201,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="8"/>
+      <c r="A25" s="7"/>
       <c r="B25" s="4" t="s">
         <v>54</v>
       </c>
@@ -1232,7 +1219,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="8"/>
+      <c r="A26" s="7"/>
       <c r="B26" s="4" t="s">
         <v>55</v>
       </c>

</xml_diff>

<commit_message>
Added form for demontstration purposes. Cleaned up CSS file.
</commit_message>
<xml_diff>
--- a/GUIs/todo.xlsx
+++ b/GUIs/todo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saad/Desktop/nasaDataViz/NASA/GUIs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7695B8D7-2952-2F4F-B853-37C8EF743FC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{997C4984-C522-8A4B-932A-7A2F967DA81F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17060" yWindow="460" windowWidth="11740" windowHeight="16220" xr2:uid="{18DB9649-71BC-4344-B476-FE1CADB6EB15}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="11740" windowHeight="16220" xr2:uid="{18DB9649-71BC-4344-B476-FE1CADB6EB15}"/>
   </bookViews>
   <sheets>
     <sheet name="MCP" sheetId="1" r:id="rId1"/>
@@ -767,8 +767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54B38FCA-31BC-F248-B08A-2E75EBF689E8}">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1201,7 +1201,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="7"/>
+      <c r="A25" s="5"/>
       <c r="B25" s="4" t="s">
         <v>54</v>
       </c>
@@ -1219,7 +1219,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="7"/>
+      <c r="A26" s="5"/>
       <c r="B26" s="4" t="s">
         <v>55</v>
       </c>

</xml_diff>